<commit_message>
added car and sar and corrected the files
</commit_message>
<xml_diff>
--- a/all_variables.xlsx
+++ b/all_variables.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\x\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EconometricsProject\Spacial-Econometrics-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5133CE08-E9D8-44AE-BE8E-162FB0054CEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="11138" yWindow="2910" windowWidth="16200" windowHeight="9308" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -29,25 +30,25 @@
     <t>Code</t>
   </si>
   <si>
-    <t>Crimes</t>
+    <t>crimes</t>
   </si>
   <si>
-    <t>social_services_users</t>
+    <t>ssusers</t>
   </si>
   <si>
-    <t>Population Density</t>
+    <t>popdens</t>
   </si>
   <si>
-    <t>Average_Monthly_Gross_Wages_and_Salaries</t>
+    <t>avgsal</t>
   </si>
   <si>
-    <t>Unemployment</t>
+    <t>unemp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -173,15 +174,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="[StdExit()] 2 2" xfId="3"/>
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
-    <cellStyle name="Normalny 2 2" xfId="1"/>
-    <cellStyle name="Normalny 3" xfId="2"/>
+    <cellStyle name="[StdExit()] 2 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny 2 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normalny 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -458,16 +459,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -487,7 +488,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>2201</v>
       </c>
@@ -507,7 +508,7 @@
         <v>2907</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>2202</v>
       </c>
@@ -527,7 +528,7 @@
         <v>3213</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>2203</v>
       </c>
@@ -547,7 +548,7 @@
         <v>1883</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>2204</v>
       </c>
@@ -567,7 +568,7 @@
         <v>1718</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>2205</v>
       </c>
@@ -587,7 +588,7 @@
         <v>1490</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>2206</v>
       </c>
@@ -607,7 +608,7 @@
         <v>1829</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>2207</v>
       </c>
@@ -627,7 +628,7 @@
         <v>1720</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>2208</v>
       </c>
@@ -647,7 +648,7 @@
         <v>1899</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>2209</v>
       </c>
@@ -667,7 +668,7 @@
         <v>2203</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>2210</v>
       </c>
@@ -687,7 +688,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>2211</v>
       </c>
@@ -707,7 +708,7 @@
         <v>1950</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>2212</v>
       </c>
@@ -727,7 +728,7 @@
         <v>2289</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>2213</v>
       </c>
@@ -747,7 +748,7 @@
         <v>2508</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>2214</v>
       </c>
@@ -767,7 +768,7 @@
         <v>2815</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>2215</v>
       </c>
@@ -787,7 +788,7 @@
         <v>3999</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>2216</v>
       </c>
@@ -807,7 +808,7 @@
         <v>1113</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>2261</v>
       </c>
@@ -827,7 +828,7 @@
         <v>6552</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>2262</v>
       </c>
@@ -847,7 +848,7 @@
         <v>2779</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>2263</v>
       </c>
@@ -867,7 +868,7 @@
         <v>1369</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>2264</v>
       </c>

</xml_diff>

<commit_message>
Population and unemp. rates added
</commit_message>
<xml_diff>
--- a/all_variables.xlsx
+++ b/all_variables.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EconometricsProject\Spacial-Econometrics-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\x\Desktop\Spatial econometrics\Spacial-Econometrics-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5133CE08-E9D8-44AE-BE8E-162FB0054CEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11138" yWindow="2910" windowWidth="16200" windowHeight="9308" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11145" yWindow="2910" windowWidth="16200" windowHeight="9315"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Code</t>
   </si>
@@ -44,15 +43,18 @@
   <si>
     <t>unemp</t>
   </si>
+  <si>
+    <t>poplation</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,25 +87,6 @@
     <font>
       <sz val="10"/>
       <name val="Arial CE"/>
-      <charset val="238"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="238"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="238"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="6"/>
-      <name val="Arial"/>
-      <family val="2"/>
       <charset val="238"/>
     </font>
   </fonts>
@@ -145,24 +128,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -177,12 +149,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="[StdExit()] 2 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normalny 2 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normalny 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="[StdExit()] 2 2" xfId="3"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny 2 2" xfId="1"/>
+    <cellStyle name="Normalny 3" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -459,433 +445,496 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G1" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>2201</v>
       </c>
       <c r="B2" s="3">
         <v>330</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="8">
         <v>5</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="9">
         <v>36</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="10">
         <v>4214.6899999999996</v>
       </c>
-      <c r="F2" s="8">
-        <v>2907</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F2" s="11">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="G2" s="9">
+        <v>79299</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2202</v>
       </c>
       <c r="B3" s="3">
         <v>658</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="8">
         <v>3.6</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="9">
         <v>72</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="12">
         <v>3761.95</v>
       </c>
-      <c r="F3" s="8">
-        <v>3213</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F3" s="11">
+        <v>8.6</v>
+      </c>
+      <c r="G3" s="9">
+        <v>97551</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2203</v>
       </c>
       <c r="B4" s="3">
         <v>264</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="8">
         <v>4.0999999999999996</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="9">
         <v>36</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="12">
         <v>3979.2</v>
       </c>
-      <c r="F4" s="8">
-        <v>1883</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F4" s="11">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="G4" s="9">
+        <v>56370</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2204</v>
       </c>
       <c r="B5" s="3">
         <v>1393</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="8">
         <v>2.2999999999999998</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="9">
         <v>146</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="10">
         <v>4438.8599999999997</v>
       </c>
-      <c r="F5" s="8">
-        <v>1718</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F5" s="11">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="G5" s="9">
+        <v>116199</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2205</v>
       </c>
       <c r="B6" s="3">
         <v>819</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="8">
         <v>3.9</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="9">
         <v>122</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="10">
         <v>3957.61</v>
       </c>
-      <c r="F6" s="8">
-        <v>1490</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F6" s="11">
+        <v>2.9</v>
+      </c>
+      <c r="G6" s="9">
+        <v>136619</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2206</v>
       </c>
       <c r="B7" s="3">
         <v>416</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="8">
         <v>5.7</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="9">
         <v>62</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="12">
         <v>3720.35</v>
       </c>
-      <c r="F7" s="8">
-        <v>1829</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F7" s="11">
+        <v>6.7</v>
+      </c>
+      <c r="G7" s="9">
+        <v>72528</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>2207</v>
       </c>
       <c r="B8" s="3">
         <v>560</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="8">
         <v>5</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="9">
         <v>100</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="10">
         <v>4362.3599999999997</v>
       </c>
-      <c r="F8" s="8">
-        <v>1720</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F8" s="11">
+        <v>5.5</v>
+      </c>
+      <c r="G8" s="9">
+        <v>83291</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>2208</v>
       </c>
       <c r="B9" s="3">
         <v>829</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="8">
         <v>5</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="9">
         <v>94</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="10">
         <v>4203.78</v>
       </c>
-      <c r="F9" s="8">
-        <v>1899</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F9" s="11">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="G9" s="9">
+        <v>66280</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>2209</v>
       </c>
       <c r="B10" s="3">
         <v>472</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="8">
         <v>4.8</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="9">
         <v>129</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="10">
         <v>3868.76</v>
       </c>
-      <c r="F10" s="8">
-        <v>2203</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F10" s="11">
+        <v>12.6</v>
+      </c>
+      <c r="G10" s="9">
+        <v>63748</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>2210</v>
       </c>
       <c r="B11" s="3">
         <v>281</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="8">
         <v>4.7</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="9">
         <v>53</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="10">
         <v>4065.87</v>
       </c>
-      <c r="F11" s="8">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F11" s="11">
+        <v>13.2</v>
+      </c>
+      <c r="G11" s="9">
+        <v>35746</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>2211</v>
       </c>
       <c r="B12" s="3">
         <v>584</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="8">
         <v>2.2999999999999998</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="9">
         <v>148</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="10">
         <v>4198.7700000000004</v>
       </c>
-      <c r="F12" s="8">
-        <v>1950</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F12" s="11">
+        <v>7.1</v>
+      </c>
+      <c r="G12" s="9">
+        <v>85726</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>2212</v>
       </c>
       <c r="B13" s="3">
         <v>619</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="8">
         <v>5</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="9">
         <v>43</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="10">
         <v>4149.8599999999997</v>
       </c>
-      <c r="F13" s="8">
-        <v>2289</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F13" s="11">
+        <v>6.9</v>
+      </c>
+      <c r="G13" s="9">
+        <v>98816</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>2213</v>
       </c>
       <c r="B14" s="3">
         <v>1099</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="8">
         <v>3.6</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="9">
         <v>95</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="10">
         <v>4323.8</v>
       </c>
-      <c r="F14" s="8">
-        <v>2508</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F14" s="11">
+        <v>5.6</v>
+      </c>
+      <c r="G14" s="9">
+        <v>128004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>2214</v>
       </c>
       <c r="B15" s="3">
         <v>1031</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="8">
         <v>3.7</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="9">
         <v>166</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="10">
         <v>4392.16</v>
       </c>
-      <c r="F15" s="8">
-        <v>2815</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F15" s="11">
+        <v>6.6</v>
+      </c>
+      <c r="G15" s="9">
+        <v>115876</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>2215</v>
       </c>
       <c r="B16" s="3">
         <v>1805</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="8">
         <v>3.4</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="9">
         <v>168</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="10">
         <v>4046.77</v>
       </c>
-      <c r="F16" s="8">
-        <v>3999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F16" s="11">
+        <v>6.5</v>
+      </c>
+      <c r="G16" s="9">
+        <v>215908</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>2216</v>
       </c>
       <c r="B17" s="3">
         <v>160</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="8">
         <v>6.6</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="9">
         <v>57</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="10">
         <v>3982.12</v>
       </c>
-      <c r="F17" s="8">
-        <v>1113</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F17" s="11">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="G17" s="9">
+        <v>41569</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>2261</v>
       </c>
       <c r="B18" s="3">
         <v>6803</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="8">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="9">
         <v>1781</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="10">
         <v>5642</v>
       </c>
-      <c r="F18" s="8">
-        <v>6552</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F18" s="11">
+        <v>2.6</v>
+      </c>
+      <c r="G18" s="9">
+        <v>466631</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>2262</v>
       </c>
       <c r="B19" s="3">
         <v>3508</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="8">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="9">
         <v>1823</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="10">
         <v>5347.46</v>
       </c>
-      <c r="F19" s="8">
-        <v>2779</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F19" s="11">
+        <v>2.5</v>
+      </c>
+      <c r="G19" s="9">
+        <v>246309</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>2263</v>
       </c>
       <c r="B20" s="3">
         <v>966</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="8">
         <v>3.1</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="9">
         <v>2109</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="10">
         <v>4057.24</v>
       </c>
-      <c r="F20" s="8">
-        <v>1369</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F20" s="11">
+        <v>3.5</v>
+      </c>
+      <c r="G20" s="9">
+        <v>91007</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>2264</v>
       </c>
       <c r="B21" s="3">
         <v>761</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="8">
         <v>1.4</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="9">
         <v>2086</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="10">
         <v>5700.74</v>
       </c>
-      <c r="F21" s="8">
-        <v>346</v>
+      <c r="F21" s="11">
+        <v>1.8</v>
+      </c>
+      <c r="G21" s="9">
+        <v>36046</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added rate of crimes
</commit_message>
<xml_diff>
--- a/all_variables.xlsx
+++ b/all_variables.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\x\Desktop\Spatial econometrics\Spacial-Econometrics-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EconometricsProject\Spacial-Econometrics-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D31222C5-9847-4D48-914B-905079F7A0C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11145" yWindow="2910" windowWidth="16200" windowHeight="9315"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Code</t>
   </si>
@@ -33,9 +34,6 @@
   </si>
   <si>
     <t>ssusers</t>
-  </si>
-  <si>
-    <t>popdens</t>
   </si>
   <si>
     <t>avgsal</t>
@@ -50,7 +48,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -128,7 +126,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -156,19 +154,16 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="[StdExit()] 2 2" xfId="3"/>
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
-    <cellStyle name="Normalny 2 2" xfId="1"/>
-    <cellStyle name="Normalny 3" xfId="2"/>
+    <cellStyle name="[StdExit()] 2 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny 2 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normalny 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -445,16 +440,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -464,20 +459,17 @@
       <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>2201</v>
       </c>
@@ -487,20 +479,17 @@
       <c r="C2" s="8">
         <v>5</v>
       </c>
-      <c r="D2" s="9">
-        <v>36</v>
-      </c>
-      <c r="E2" s="10">
+      <c r="D2" s="10">
         <v>4214.6899999999996</v>
       </c>
-      <c r="F2" s="11">
+      <c r="E2" s="11">
         <v>9.6999999999999993</v>
       </c>
-      <c r="G2" s="9">
+      <c r="F2" s="9">
         <v>79299</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>2202</v>
       </c>
@@ -510,20 +499,17 @@
       <c r="C3" s="8">
         <v>3.6</v>
       </c>
-      <c r="D3" s="9">
-        <v>72</v>
-      </c>
-      <c r="E3" s="12">
+      <c r="D3" s="12">
         <v>3761.95</v>
       </c>
-      <c r="F3" s="11">
+      <c r="E3" s="11">
         <v>8.6</v>
       </c>
-      <c r="G3" s="9">
+      <c r="F3" s="9">
         <v>97551</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>2203</v>
       </c>
@@ -533,20 +519,17 @@
       <c r="C4" s="8">
         <v>4.0999999999999996</v>
       </c>
-      <c r="D4" s="9">
-        <v>36</v>
-      </c>
-      <c r="E4" s="12">
+      <c r="D4" s="12">
         <v>3979.2</v>
       </c>
-      <c r="F4" s="11">
+      <c r="E4" s="11">
         <v>9.8000000000000007</v>
       </c>
-      <c r="G4" s="9">
+      <c r="F4" s="9">
         <v>56370</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>2204</v>
       </c>
@@ -556,20 +539,17 @@
       <c r="C5" s="8">
         <v>2.2999999999999998</v>
       </c>
-      <c r="D5" s="9">
-        <v>146</v>
-      </c>
-      <c r="E5" s="10">
+      <c r="D5" s="10">
         <v>4438.8599999999997</v>
       </c>
-      <c r="F5" s="11">
+      <c r="E5" s="11">
         <v>4.0999999999999996</v>
       </c>
-      <c r="G5" s="9">
+      <c r="F5" s="9">
         <v>116199</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>2205</v>
       </c>
@@ -579,20 +559,17 @@
       <c r="C6" s="8">
         <v>3.9</v>
       </c>
-      <c r="D6" s="9">
-        <v>122</v>
-      </c>
-      <c r="E6" s="10">
+      <c r="D6" s="10">
         <v>3957.61</v>
       </c>
-      <c r="F6" s="11">
+      <c r="E6" s="11">
         <v>2.9</v>
       </c>
-      <c r="G6" s="9">
+      <c r="F6" s="9">
         <v>136619</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>2206</v>
       </c>
@@ -602,20 +579,17 @@
       <c r="C7" s="8">
         <v>5.7</v>
       </c>
-      <c r="D7" s="9">
-        <v>62</v>
-      </c>
-      <c r="E7" s="12">
+      <c r="D7" s="12">
         <v>3720.35</v>
       </c>
-      <c r="F7" s="11">
+      <c r="E7" s="11">
         <v>6.7</v>
       </c>
-      <c r="G7" s="9">
+      <c r="F7" s="9">
         <v>72528</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>2207</v>
       </c>
@@ -625,20 +599,17 @@
       <c r="C8" s="8">
         <v>5</v>
       </c>
-      <c r="D8" s="9">
-        <v>100</v>
-      </c>
-      <c r="E8" s="10">
+      <c r="D8" s="10">
         <v>4362.3599999999997</v>
       </c>
-      <c r="F8" s="11">
+      <c r="E8" s="11">
         <v>5.5</v>
       </c>
-      <c r="G8" s="9">
+      <c r="F8" s="9">
         <v>83291</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>2208</v>
       </c>
@@ -648,20 +619,17 @@
       <c r="C9" s="8">
         <v>5</v>
       </c>
-      <c r="D9" s="9">
-        <v>94</v>
-      </c>
-      <c r="E9" s="10">
+      <c r="D9" s="10">
         <v>4203.78</v>
       </c>
-      <c r="F9" s="11">
+      <c r="E9" s="11">
         <v>8.8000000000000007</v>
       </c>
-      <c r="G9" s="9">
+      <c r="F9" s="9">
         <v>66280</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>2209</v>
       </c>
@@ -671,20 +639,17 @@
       <c r="C10" s="8">
         <v>4.8</v>
       </c>
-      <c r="D10" s="9">
-        <v>129</v>
-      </c>
-      <c r="E10" s="10">
+      <c r="D10" s="10">
         <v>3868.76</v>
       </c>
-      <c r="F10" s="11">
+      <c r="E10" s="11">
         <v>12.6</v>
       </c>
-      <c r="G10" s="9">
+      <c r="F10" s="9">
         <v>63748</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>2210</v>
       </c>
@@ -694,20 +659,17 @@
       <c r="C11" s="8">
         <v>4.7</v>
       </c>
-      <c r="D11" s="9">
-        <v>53</v>
-      </c>
-      <c r="E11" s="10">
+      <c r="D11" s="10">
         <v>4065.87</v>
       </c>
-      <c r="F11" s="11">
+      <c r="E11" s="11">
         <v>13.2</v>
       </c>
-      <c r="G11" s="9">
+      <c r="F11" s="9">
         <v>35746</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>2211</v>
       </c>
@@ -717,20 +679,17 @@
       <c r="C12" s="8">
         <v>2.2999999999999998</v>
       </c>
-      <c r="D12" s="9">
-        <v>148</v>
-      </c>
-      <c r="E12" s="10">
+      <c r="D12" s="10">
         <v>4198.7700000000004</v>
       </c>
-      <c r="F12" s="11">
+      <c r="E12" s="11">
         <v>7.1</v>
       </c>
-      <c r="G12" s="9">
+      <c r="F12" s="9">
         <v>85726</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>2212</v>
       </c>
@@ -740,20 +699,17 @@
       <c r="C13" s="8">
         <v>5</v>
       </c>
-      <c r="D13" s="9">
-        <v>43</v>
-      </c>
-      <c r="E13" s="10">
+      <c r="D13" s="10">
         <v>4149.8599999999997</v>
       </c>
-      <c r="F13" s="11">
+      <c r="E13" s="11">
         <v>6.9</v>
       </c>
-      <c r="G13" s="9">
+      <c r="F13" s="9">
         <v>98816</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>2213</v>
       </c>
@@ -763,20 +719,17 @@
       <c r="C14" s="8">
         <v>3.6</v>
       </c>
-      <c r="D14" s="9">
-        <v>95</v>
-      </c>
-      <c r="E14" s="10">
+      <c r="D14" s="10">
         <v>4323.8</v>
       </c>
-      <c r="F14" s="11">
+      <c r="E14" s="11">
         <v>5.6</v>
       </c>
-      <c r="G14" s="9">
+      <c r="F14" s="9">
         <v>128004</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>2214</v>
       </c>
@@ -786,20 +739,17 @@
       <c r="C15" s="8">
         <v>3.7</v>
       </c>
-      <c r="D15" s="9">
-        <v>166</v>
-      </c>
-      <c r="E15" s="10">
+      <c r="D15" s="10">
         <v>4392.16</v>
       </c>
-      <c r="F15" s="11">
+      <c r="E15" s="11">
         <v>6.6</v>
       </c>
-      <c r="G15" s="9">
+      <c r="F15" s="9">
         <v>115876</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>2215</v>
       </c>
@@ -809,20 +759,17 @@
       <c r="C16" s="8">
         <v>3.4</v>
       </c>
-      <c r="D16" s="9">
-        <v>168</v>
-      </c>
-      <c r="E16" s="10">
+      <c r="D16" s="10">
         <v>4046.77</v>
       </c>
-      <c r="F16" s="11">
+      <c r="E16" s="11">
         <v>6.5</v>
       </c>
-      <c r="G16" s="9">
+      <c r="F16" s="9">
         <v>215908</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>2216</v>
       </c>
@@ -832,20 +779,17 @@
       <c r="C17" s="8">
         <v>6.6</v>
       </c>
-      <c r="D17" s="9">
-        <v>57</v>
-      </c>
-      <c r="E17" s="10">
+      <c r="D17" s="10">
         <v>3982.12</v>
       </c>
-      <c r="F17" s="11">
+      <c r="E17" s="11">
         <v>9.6999999999999993</v>
       </c>
-      <c r="G17" s="9">
+      <c r="F17" s="9">
         <v>41569</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>2261</v>
       </c>
@@ -855,20 +799,17 @@
       <c r="C18" s="8">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D18" s="9">
-        <v>1781</v>
-      </c>
-      <c r="E18" s="10">
+      <c r="D18" s="10">
         <v>5642</v>
       </c>
-      <c r="F18" s="11">
+      <c r="E18" s="11">
         <v>2.6</v>
       </c>
-      <c r="G18" s="9">
+      <c r="F18" s="9">
         <v>466631</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>2262</v>
       </c>
@@ -878,20 +819,17 @@
       <c r="C19" s="8">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D19" s="9">
-        <v>1823</v>
-      </c>
-      <c r="E19" s="10">
+      <c r="D19" s="10">
         <v>5347.46</v>
       </c>
-      <c r="F19" s="11">
+      <c r="E19" s="11">
         <v>2.5</v>
       </c>
-      <c r="G19" s="9">
+      <c r="F19" s="9">
         <v>246309</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>2263</v>
       </c>
@@ -901,20 +839,17 @@
       <c r="C20" s="8">
         <v>3.1</v>
       </c>
-      <c r="D20" s="9">
-        <v>2109</v>
-      </c>
-      <c r="E20" s="10">
+      <c r="D20" s="10">
         <v>4057.24</v>
       </c>
-      <c r="F20" s="11">
+      <c r="E20" s="11">
         <v>3.5</v>
       </c>
-      <c r="G20" s="9">
+      <c r="F20" s="9">
         <v>91007</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>2264</v>
       </c>
@@ -924,16 +859,13 @@
       <c r="C21" s="8">
         <v>1.4</v>
       </c>
-      <c r="D21" s="9">
-        <v>2086</v>
-      </c>
-      <c r="E21" s="10">
+      <c r="D21" s="10">
         <v>5700.74</v>
       </c>
-      <c r="F21" s="11">
+      <c r="E21" s="11">
         <v>1.8</v>
       </c>
-      <c r="G21" s="9">
+      <c r="F21" s="9">
         <v>36046</v>
       </c>
     </row>

</xml_diff>